<commit_message>
Add float pattern and update example
Signed-off-by: Allen Ni <724330304@qq.com>
</commit_message>
<xml_diff>
--- a/input_example.xlsx
+++ b/input_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allen/Codes/DataGenerator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5CAB3A-B797-E74C-AA9E-B33C8C189567}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A5BD7A-EFC4-F744-82B3-F58C9BE1F0BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{228639C1-B127-C84B-8238-B7752E23BC74}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>CMBB+ID</t>
+  </si>
+  <si>
+    <t>%.2f</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,6 +824,12 @@
       <c r="L6" t="s">
         <v>30</v>
       </c>
+      <c r="M6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">

</xml_diff>